<commit_message>
fixed alot of things, but made another problem .. COLONS
</commit_message>
<xml_diff>
--- a/dialogue/Weather Tweets/Weather.xlsx
+++ b/dialogue/Weather Tweets/Weather.xlsx
@@ -63,9 +63,6 @@
     <t>~</t>
   </si>
   <si>
-    <t>cityName</t>
-  </si>
-  <si>
     <t>city_output</t>
   </si>
   <si>
@@ -165,18 +162,12 @@
     <t>random</t>
   </si>
   <si>
-    <t>It is $tempurature_other$°C in $cityName_other$.</t>
-  </si>
-  <si>
     <t>The sun should set at $sunset_other$ tonight.</t>
   </si>
   <si>
     <t>The air is $humidity_other$% water at the moment.</t>
   </si>
   <si>
-    <t>It looks like it's $description_other$ here in $cityName_other$</t>
-  </si>
-  <si>
     <t>My head hurts .. It's probably because the pressure is $pressure_other$ hPa.</t>
   </si>
   <si>
@@ -186,10 +177,19 @@
     <t>kTemp</t>
   </si>
   <si>
-    <t>kelvinTemp</t>
-  </si>
-  <si>
-    <t>In $cityName_other$ it's $tempurature_other$°C .. THAT'S $kelvinTemp_other% IN KELVIN.</t>
+    <t>kelvintemp</t>
+  </si>
+  <si>
+    <t>It looks like it's $description_other$ here in $cityname_other$</t>
+  </si>
+  <si>
+    <t>cityname</t>
+  </si>
+  <si>
+    <t>It is $tempurature_other$°C in $cityname_other$.</t>
+  </si>
+  <si>
+    <t>In $cityname_other$ it's $tempurature_other$°C .. THAT'S $kelvintemp_other$ IN KELVIN.</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -590,10 +590,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -601,27 +601,27 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -629,27 +629,27 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -657,27 +657,27 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
         <v>37</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -685,47 +685,47 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -738,13 +738,13 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -752,13 +752,13 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -766,13 +766,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -780,13 +780,13 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
         <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -794,13 +794,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
         <v>43</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -808,13 +808,13 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
         <v>29</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -822,13 +822,13 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -836,13 +836,13 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -850,13 +850,13 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -864,13 +864,13 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -878,13 +878,13 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -892,10 +892,10 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
weather tweets are now working properly. had to deal with the stupid issue of something not working. I think it was related to cleverscript and how they process characters
</commit_message>
<xml_diff>
--- a/dialogue/Weather Tweets/Weather.xlsx
+++ b/dialogue/Weather Tweets/Weather.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
   <si>
     <t>Type</t>
   </si>
@@ -190,13 +190,16 @@
   </si>
   <si>
     <t>In $cityname_other$ it's $tempurature_other$°C .. THAT'S $kelvintemp_other$ IN KELVIN.</t>
+  </si>
+  <si>
+    <t>The sun rose at $sunrise_other$ this morning!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -211,6 +214,12 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -245,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -253,6 +262,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,11 +545,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -546,7 +558,7 @@
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="61.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
@@ -714,37 +726,28 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
-        <v>48</v>
+      <c r="D12" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -752,13 +755,13 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -766,13 +769,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -780,13 +783,13 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -794,13 +797,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -808,13 +811,13 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -822,13 +825,13 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -836,13 +839,13 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -850,13 +853,13 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -864,13 +867,13 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -878,13 +881,13 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -892,19 +895,34 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
         <v>20</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>